<commit_message>
Ergänzung Punkt Aufnahme Visual Studio in Objekte
</commit_message>
<xml_diff>
--- a/8. Harmonising standards/01_Project organisation/03_Project Documentation/ReleasePlan_Template ProjectDocu.xlsx
+++ b/8. Harmonising standards/01_Project organisation/03_Project Documentation/ReleasePlan_Template ProjectDocu.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20827"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E97302EA-0748-4511-9C09-FAA6658772DA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{161690FA-8B75-4198-84D8-4415A6D1BBE1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12000" windowHeight="4725" tabRatio="837" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
   <si>
     <t>SAXESS Software GmbH</t>
   </si>
@@ -137,6 +137,9 @@
   </si>
   <si>
     <t>Links in Prozedurobjekten auf Statuskreis legen und nicht auf gesamtes Objekt</t>
+  </si>
+  <si>
+    <t>Objekt Visual Studio in Corporate Design aufnehmen</t>
   </si>
 </sst>
 </file>
@@ -355,7 +358,31 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -625,6 +652,252 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>2428875</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>600074</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>9523</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="4" name="Gruppieren 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32897A1D-73A3-4E1A-B49B-8FF4E0237579}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="15125700" y="8086725"/>
+          <a:ext cx="1552574" cy="771523"/>
+          <a:chOff x="5819775" y="28317826"/>
+          <a:chExt cx="1552574" cy="771523"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="5" name="Gruppieren 4">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8327F08F-26E2-4AD0-8A53-706A28E13AE8}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="5819775" y="28394024"/>
+            <a:ext cx="1552574" cy="695325"/>
+            <a:chOff x="1676400" y="2714625"/>
+            <a:chExt cx="1552574" cy="695325"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="7" name="Rechteck 6">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7938177-6D98-475A-AFC3-EDB86AD11DAD}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1676400" y="2867025"/>
+              <a:ext cx="1552574" cy="542925"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:r>
+                <a:rPr lang="de-DE" sz="900" b="1">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t>Visual</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="900" b="1" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t> Studio</a:t>
+              </a:r>
+              <a:endParaRPr lang="de-DE" sz="900" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:r>
+                <a:rPr lang="de-DE" sz="800" b="0">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t>Entwicklungsumgebung Tabular Model</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="8" name="Textfeld 7">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BC35E26-8D2B-4CF5-B555-A7125CE9D576}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1933575" y="2714625"/>
+              <a:ext cx="1181100" cy="122590"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525" cmpd="sng">
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="de-DE" sz="900">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t>Microsoft Visual Studio</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:endParaRPr lang="de-DE" sz="900">
+                <a:solidFill>
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="6" name="Grafik 5">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75D11A4A-3EED-4684-9402-4E437DCD2C56}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5838825" y="28317826"/>
+            <a:ext cx="209550" cy="209550"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -900,9 +1173,9 @@
   <dimension ref="A1:BB315"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="7" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H33" sqref="H33"/>
-      <selection pane="bottomLeft" activeCell="N45" sqref="N45"/>
+      <selection pane="bottomLeft" activeCell="N51" sqref="N51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1657,13 +1930,27 @@
       <c r="N43" s="36"/>
     </row>
     <row r="44" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="C44" s="19"/>
+      <c r="B44" s="18">
+        <v>3</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>37</v>
+      </c>
       <c r="I44" s="20"/>
-      <c r="J44" s="20"/>
-      <c r="K44" s="20"/>
-      <c r="L44" s="22"/>
+      <c r="J44" s="20">
+        <v>100</v>
+      </c>
+      <c r="K44" s="20">
+        <f>I44/100*(100-J44)</f>
+        <v>0</v>
+      </c>
+      <c r="L44" s="22" t="s">
+        <v>12</v>
+      </c>
       <c r="M44" s="22"/>
-      <c r="N44" s="33"/>
+      <c r="N44" s="36" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="45" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C45" s="19"/>
@@ -1672,7 +1959,9 @@
       <c r="K45" s="20"/>
       <c r="L45" s="22"/>
       <c r="M45" s="22"/>
-      <c r="N45" s="33"/>
+      <c r="N45" s="36" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="46" spans="2:14" s="38" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25"/>
     <row r="47" spans="2:14" x14ac:dyDescent="0.25">
@@ -3416,7 +3705,15 @@
   <mergeCells count="1">
     <mergeCell ref="A46:XFD46"/>
   </mergeCells>
-  <conditionalFormatting sqref="M27 M9:M10 M33:M40 M16 M22:M25 M47:M1005 M43:M45">
+  <conditionalFormatting sqref="M27 M9:M10 M33:M40 M16 M22:M25 M47:M1005 M43">
+    <cfRule type="cellIs" dxfId="13" priority="15" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="16" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M26">
     <cfRule type="cellIs" dxfId="11" priority="13" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
@@ -3424,15 +3721,15 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M26">
-    <cfRule type="cellIs" dxfId="9" priority="11" operator="greaterThan">
+  <conditionalFormatting sqref="M28:M32">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M28:M32">
+  <conditionalFormatting sqref="M11:M15">
     <cfRule type="cellIs" dxfId="7" priority="7" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
@@ -3440,7 +3737,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M11:M15">
+  <conditionalFormatting sqref="M17:M21">
     <cfRule type="cellIs" dxfId="5" priority="5" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
@@ -3448,7 +3745,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M17:M21">
+  <conditionalFormatting sqref="M41:M42">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
@@ -3456,7 +3753,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M41:M42">
+  <conditionalFormatting sqref="M44:M45">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>

</xml_diff>

<commit_message>
Ergänzung Punkte Symbol Speichern, Gruppierung
</commit_message>
<xml_diff>
--- a/8. Harmonising standards/01_Project organisation/03_Project Documentation/ReleasePlan_Template ProjectDocu.xlsx
+++ b/8. Harmonising standards/01_Project organisation/03_Project Documentation/ReleasePlan_Template ProjectDocu.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20827"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{161690FA-8B75-4198-84D8-4415A6D1BBE1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{324CB801-EE65-4533-9845-76D9ADEBFAD8}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12000" windowHeight="4725" tabRatio="837" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
   <si>
     <t>SAXESS Software GmbH</t>
   </si>
@@ -140,6 +140,15 @@
   </si>
   <si>
     <t>Objekt Visual Studio in Corporate Design aufnehmen</t>
+  </si>
+  <si>
+    <t>Ergänzen eines Speichersymbols für Prozessbeschreibung</t>
+  </si>
+  <si>
+    <t>Gruppierung bei Prozedur mit API-Anpassung (API-Symbol kopiert es nicht mit)</t>
+  </si>
+  <si>
+    <t>Gruppierung bei Prozedur Kundenerweiterung (Parameter kopiert es nicht mit)</t>
   </si>
 </sst>
 </file>
@@ -348,8 +357,8 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -358,7 +367,79 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="20">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -900,6 +981,830 @@
     </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>2647950</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>3257549</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>86098</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Grafik 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3F6E2D3-CFC4-4251-ACA8-60BEE2C17A53}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="15344775" y="9105900"/>
+          <a:ext cx="609599" cy="400423"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>2438400</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>59025</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>109894</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="10" name="Gruppieren 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9CA32C2-A2A7-4601-92A2-C2609939D83A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="15135225" y="9686925"/>
+          <a:ext cx="1764000" cy="795694"/>
+          <a:chOff x="2390775" y="10134614"/>
+          <a:chExt cx="1764000" cy="795694"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="11" name="Gruppieren 10">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02313153-602F-44F6-BCA5-CE03F4913D2C}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="2390775" y="10134614"/>
+            <a:ext cx="1764000" cy="795694"/>
+            <a:chOff x="7953375" y="9620250"/>
+            <a:chExt cx="1764000" cy="633410"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="13" name="Textfeld 12">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71861326-A24E-422E-831F-11FAB6C9414C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8143875" y="9667875"/>
+              <a:ext cx="1181100" cy="152400"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:alpha val="80000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="9525" cmpd="sng">
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="de-DE" sz="900">
+                  <a:solidFill>
+                    <a:srgbClr val="69B42E"/>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t>DataFactory Prozedur </a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="14" name="Rechteck 13">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{112433C8-D09A-4F54-9A9C-DD782E5E2C1F}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7962900" y="9620250"/>
+              <a:ext cx="122726" cy="168519"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="36000" tIns="36000" rIns="36000" bIns="36000" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="de-DE" sz="900">
+                  <a:solidFill>
+                    <a:srgbClr val="69B42E"/>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t>P</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="15" name="Textfeld 14">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{502C3D94-86D0-44CE-B6F3-C230869225AF}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7953375" y="9823794"/>
+              <a:ext cx="1764000" cy="429866"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:alpha val="80000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="9525" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="36000" tIns="36000" rIns="36000" bIns="36000" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="de-DE" sz="900" b="1">
+                  <a:solidFill>
+                    <a:srgbClr val="69B42E"/>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t>dbo.sx_pf_COPY_Factory</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:r>
+                <a:rPr lang="de-DE" sz="800">
+                  <a:solidFill>
+                    <a:srgbClr val="69B42E"/>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t>Kopiert eine Factory</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="12" name="Rechteck 11">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC9560ED-6E02-47C2-818D-0528CC57BA07}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3743325" y="10706101"/>
+            <a:ext cx="371475" cy="190500"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="accent4">
+              <a:lumMod val="20000"/>
+              <a:lumOff val="80000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:prstDash val="dash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="de-DE" sz="900" b="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>API</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>2219325</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>86283</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="17" name="Gruppieren 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4067E23B-7DCE-46D9-BAFF-74A59E6EF245}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="14916150" y="10791825"/>
+          <a:ext cx="2486025" cy="810183"/>
+          <a:chOff x="266700" y="8058186"/>
+          <a:chExt cx="2486025" cy="810183"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="18" name="Gruppieren 17">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6F8D34E-C9BB-4C19-B8BA-270DAACFE0D2}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="266700" y="8124825"/>
+            <a:ext cx="2340000" cy="743544"/>
+            <a:chOff x="1733550" y="3286125"/>
+            <a:chExt cx="2340000" cy="743544"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:grpSp>
+          <xdr:nvGrpSpPr>
+            <xdr:cNvPr id="22" name="Gruppieren 21">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F9B8A5F-3EE1-4393-BE54-A20E668564EB}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGrpSpPr/>
+          </xdr:nvGrpSpPr>
+          <xdr:grpSpPr>
+            <a:xfrm>
+              <a:off x="1733550" y="3286125"/>
+              <a:ext cx="2340000" cy="743544"/>
+              <a:chOff x="7953375" y="9620250"/>
+              <a:chExt cx="2340000" cy="743544"/>
+            </a:xfrm>
+          </xdr:grpSpPr>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="24" name="Textfeld 23">
+                <a:extLst>
+                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DAEF804C-AE88-4950-8437-5114CCFB7AD8}"/>
+                  </a:ext>
+                </a:extLst>
+              </xdr:cNvPr>
+              <xdr:cNvSpPr txBox="1"/>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="8143875" y="9667875"/>
+                <a:ext cx="1181100" cy="152400"/>
+              </a:xfrm>
+              <a:prstGeom prst="rect">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:alpha val="80000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525" cmpd="sng">
+                <a:noFill/>
+              </a:ln>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="0">
+                <a:scrgbClr r="0" g="0" b="0"/>
+              </a:lnRef>
+              <a:fillRef idx="0">
+                <a:scrgbClr r="0" g="0" b="0"/>
+              </a:fillRef>
+              <a:effectRef idx="0">
+                <a:scrgbClr r="0" g="0" b="0"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="dk1"/>
+              </a:fontRef>
+            </xdr:style>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="900">
+                    <a:solidFill>
+                      <a:schemeClr val="accent5">
+                        <a:lumMod val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Prozedur </a:t>
+                </a:r>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="25" name="Rechteck 24">
+                <a:extLst>
+                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{933C6063-7B7B-4AC7-8EC0-C1EC4E7A2612}"/>
+                  </a:ext>
+                </a:extLst>
+              </xdr:cNvPr>
+              <xdr:cNvSpPr/>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="7962900" y="9620250"/>
+                <a:ext cx="122726" cy="168519"/>
+              </a:xfrm>
+              <a:prstGeom prst="rect">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="203864"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="2">
+                <a:schemeClr val="accent1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:lnRef>
+              <a:fillRef idx="1">
+                <a:schemeClr val="accent1"/>
+              </a:fillRef>
+              <a:effectRef idx="0">
+                <a:schemeClr val="accent1"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="lt1"/>
+              </a:fontRef>
+            </xdr:style>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="36000" tIns="36000" rIns="36000" bIns="36000" rtlCol="0" anchor="ctr"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="ctr"/>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="900">
+                    <a:solidFill>
+                      <a:srgbClr val="203864"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>P</a:t>
+                </a:r>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="26" name="Textfeld 25">
+                <a:extLst>
+                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8EE4CFD-E7EE-4129-90FE-D5F046C5D409}"/>
+                  </a:ext>
+                </a:extLst>
+              </xdr:cNvPr>
+              <xdr:cNvSpPr txBox="1"/>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="7953375" y="9823794"/>
+                <a:ext cx="2340000" cy="540000"/>
+              </a:xfrm>
+              <a:prstGeom prst="rect">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:alpha val="80000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525" cmpd="sng">
+                <a:solidFill>
+                  <a:srgbClr val="203864"/>
+                </a:solidFill>
+              </a:ln>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="0">
+                <a:scrgbClr r="0" g="0" b="0"/>
+              </a:lnRef>
+              <a:fillRef idx="0">
+                <a:scrgbClr r="0" g="0" b="0"/>
+              </a:fillRef>
+              <a:effectRef idx="0">
+                <a:scrgbClr r="0" g="0" b="0"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="dk1"/>
+              </a:fontRef>
+            </xdr:style>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="36000" tIns="36000" rIns="36000" bIns="36000" rtlCol="0" anchor="t"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="900" b="1">
+                    <a:solidFill>
+                      <a:srgbClr val="203864"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>control.spPlanBudget_ArchiveCC</a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="800">
+                    <a:solidFill>
+                      <a:srgbClr val="203864"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Schreibt</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="800" baseline="0">
+                    <a:solidFill>
+                      <a:srgbClr val="203864"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t> Planwerte für bestimmten Mandanten, bestimmte Kostenstelle, Jahren, Monaten  </a:t>
+                </a:r>
+                <a:endParaRPr lang="de-DE" sz="800">
+                  <a:solidFill>
+                    <a:srgbClr val="203864"/>
+                  </a:solidFill>
+                </a:endParaRPr>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+        </xdr:grpSp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="23" name="Ellipse 22">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1678D565-BAF4-4646-9BDE-29335B9CB363}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3829050" y="3381375"/>
+              <a:ext cx="180000" cy="180000"/>
+            </a:xfrm>
+            <a:prstGeom prst="ellipse">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="de-DE" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="19" name="Gruppieren 18">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BD6E0CD-EA99-4971-BC91-C29E02C6C4B6}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="1400176" y="8058186"/>
+            <a:ext cx="1352549" cy="257155"/>
+            <a:chOff x="12773026" y="7430705"/>
+            <a:chExt cx="1352549" cy="220935"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="20" name="Textfeld 19">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F9E195CB-CC45-4DBF-953E-937761A2E38C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="12944475" y="7430705"/>
+              <a:ext cx="1181100" cy="220935"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525" cmpd="sng">
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="de-DE" sz="800">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t>Mandant,Kostentelle,</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:r>
+                <a:rPr lang="de-DE" sz="800">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t>Jahr,Monat</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="21" name="Grafik 20">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{365CEEDF-831D-4E43-A5D6-DC6067DF7305}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1"/>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+              <a:duotone>
+                <a:schemeClr val="accent3">
+                  <a:shade val="45000"/>
+                  <a:satMod val="135000"/>
+                </a:schemeClr>
+                <a:prstClr val="white"/>
+              </a:duotone>
+              <a:extLst>
+                <a:ext uri="{BEBA8EAE-BF5A-486C-A8C5-ECC9F3942E4B}">
+                  <a14:imgProps xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                    <a14:imgLayer r:embed="rId6">
+                      <a14:imgEffect>
+                        <a14:backgroundRemoval t="0" b="100000" l="0" r="100000"/>
+                      </a14:imgEffect>
+                    </a14:imgLayer>
+                  </a14:imgProps>
+                </a:ext>
+              </a:extLst>
+            </a:blip>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="12773026" y="7476992"/>
+              <a:ext cx="141914" cy="141913"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </xdr:grpSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1173,9 +2078,9 @@
   <dimension ref="A1:BB315"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="7" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H33" sqref="H33"/>
-      <selection pane="bottomLeft" activeCell="N51" sqref="N51"/>
+      <selection pane="bottomLeft" activeCell="N61" sqref="N61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1965,12 +2870,27 @@
     </row>
     <row r="46" spans="2:14" s="38" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25"/>
     <row r="47" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B47" s="18">
+        <v>4</v>
+      </c>
+      <c r="C47" s="11" t="s">
+        <v>38</v>
+      </c>
       <c r="I47" s="20"/>
-      <c r="J47" s="20"/>
-      <c r="K47" s="20"/>
-      <c r="L47" s="22"/>
+      <c r="J47" s="20">
+        <v>100</v>
+      </c>
+      <c r="K47" s="20">
+        <f>I47/100*(100-J47)</f>
+        <v>0</v>
+      </c>
+      <c r="L47" s="22" t="s">
+        <v>12</v>
+      </c>
       <c r="M47" s="22"/>
-      <c r="N47" s="33"/>
+      <c r="N47" s="36" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="48" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I48" s="20"/>
@@ -1978,9 +2898,11 @@
       <c r="K48" s="20"/>
       <c r="L48" s="22"/>
       <c r="M48" s="22"/>
-      <c r="N48" s="33"/>
-    </row>
-    <row r="49" spans="9:14" x14ac:dyDescent="0.25">
+      <c r="N48" s="36" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I49" s="20"/>
       <c r="J49" s="20"/>
       <c r="K49" s="20"/>
@@ -1988,106 +2910,145 @@
       <c r="M49" s="22"/>
       <c r="N49" s="33"/>
     </row>
-    <row r="50" spans="9:14" x14ac:dyDescent="0.25">
-      <c r="I50" s="21"/>
-      <c r="J50" s="21"/>
-      <c r="K50" s="21"/>
-      <c r="L50" s="23"/>
-      <c r="M50" s="23"/>
-      <c r="N50" s="37"/>
-    </row>
-    <row r="51" spans="9:14" x14ac:dyDescent="0.25">
-      <c r="I51" s="21"/>
-      <c r="J51" s="21"/>
-      <c r="K51" s="21"/>
-      <c r="L51" s="23"/>
-      <c r="M51" s="23"/>
-    </row>
-    <row r="52" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B50" s="18">
+        <v>5</v>
+      </c>
+      <c r="C50" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="I50" s="20"/>
+      <c r="J50" s="20">
+        <v>100</v>
+      </c>
+      <c r="K50" s="20">
+        <f>I50/100*(100-J50)</f>
+        <v>0</v>
+      </c>
+      <c r="L50" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="M50" s="22"/>
+      <c r="N50" s="36" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I51" s="20"/>
+      <c r="J51" s="20"/>
+      <c r="K51" s="20"/>
+      <c r="L51" s="22"/>
+      <c r="M51" s="22"/>
+      <c r="N51" s="36" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I52" s="21"/>
       <c r="J52" s="21"/>
       <c r="K52" s="21"/>
       <c r="L52" s="23"/>
       <c r="M52" s="23"/>
     </row>
-    <row r="53" spans="9:14" x14ac:dyDescent="0.25">
-      <c r="I53" s="21"/>
-      <c r="J53" s="21"/>
-      <c r="K53" s="21"/>
-      <c r="L53" s="23"/>
-      <c r="M53" s="23"/>
-    </row>
-    <row r="54" spans="9:14" x14ac:dyDescent="0.25">
-      <c r="I54" s="21"/>
-      <c r="J54" s="21"/>
-      <c r="K54" s="21"/>
-      <c r="L54" s="23"/>
-      <c r="M54" s="23"/>
-    </row>
-    <row r="55" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B53" s="18">
+        <v>6</v>
+      </c>
+      <c r="C53" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H53" s="37"/>
+      <c r="I53" s="20"/>
+      <c r="J53" s="20">
+        <v>100</v>
+      </c>
+      <c r="K53" s="20">
+        <f>I53/100*(100-J53)</f>
+        <v>0</v>
+      </c>
+      <c r="L53" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="M53" s="22"/>
+      <c r="N53" s="36" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="H54" s="37"/>
+      <c r="I54" s="20"/>
+      <c r="J54" s="20"/>
+      <c r="K54" s="20"/>
+      <c r="L54" s="22"/>
+      <c r="M54" s="22"/>
+      <c r="N54" s="36" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="55" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I55" s="21"/>
       <c r="J55" s="21"/>
       <c r="K55" s="21"/>
       <c r="L55" s="23"/>
       <c r="M55" s="23"/>
     </row>
-    <row r="56" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I56" s="21"/>
       <c r="J56" s="21"/>
       <c r="K56" s="21"/>
       <c r="L56" s="23"/>
       <c r="M56" s="23"/>
     </row>
-    <row r="57" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I57" s="21"/>
       <c r="J57" s="21"/>
       <c r="K57" s="21"/>
       <c r="L57" s="23"/>
       <c r="M57" s="23"/>
     </row>
-    <row r="58" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I58" s="21"/>
       <c r="J58" s="21"/>
       <c r="K58" s="21"/>
       <c r="L58" s="23"/>
       <c r="M58" s="23"/>
     </row>
-    <row r="59" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I59" s="21"/>
       <c r="J59" s="21"/>
       <c r="K59" s="21"/>
       <c r="L59" s="23"/>
       <c r="M59" s="23"/>
     </row>
-    <row r="60" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I60" s="21"/>
       <c r="J60" s="21"/>
       <c r="K60" s="21"/>
       <c r="L60" s="23"/>
       <c r="M60" s="23"/>
     </row>
-    <row r="61" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I61" s="21"/>
       <c r="J61" s="21"/>
       <c r="K61" s="21"/>
       <c r="L61" s="23"/>
       <c r="M61" s="23"/>
     </row>
-    <row r="62" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I62" s="21"/>
       <c r="J62" s="21"/>
       <c r="K62" s="21"/>
       <c r="L62" s="23"/>
       <c r="M62" s="23"/>
     </row>
-    <row r="63" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I63" s="21"/>
       <c r="J63" s="21"/>
       <c r="K63" s="21"/>
       <c r="L63" s="23"/>
       <c r="M63" s="23"/>
     </row>
-    <row r="64" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I64" s="21"/>
       <c r="J64" s="21"/>
       <c r="K64" s="21"/>
@@ -3705,23 +4666,47 @@
   <mergeCells count="1">
     <mergeCell ref="A46:XFD46"/>
   </mergeCells>
-  <conditionalFormatting sqref="M27 M9:M10 M33:M40 M16 M22:M25 M47:M1005 M43">
-    <cfRule type="cellIs" dxfId="13" priority="15" operator="greaterThan">
+  <conditionalFormatting sqref="M27 M9:M10 M33:M40 M16 M22:M25 M49 M43 M52 M55:M1005">
+    <cfRule type="cellIs" dxfId="19" priority="21" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="22" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M26">
-    <cfRule type="cellIs" dxfId="11" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="19" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="20" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M28:M32">
+    <cfRule type="cellIs" dxfId="15" priority="15" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M11:M15">
+    <cfRule type="cellIs" dxfId="13" priority="13" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M17:M21">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M41:M42">
     <cfRule type="cellIs" dxfId="9" priority="9" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
@@ -3729,7 +4714,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M11:M15">
+  <conditionalFormatting sqref="M44:M45">
     <cfRule type="cellIs" dxfId="7" priority="7" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
@@ -3737,7 +4722,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M17:M21">
+  <conditionalFormatting sqref="M47:M48">
     <cfRule type="cellIs" dxfId="5" priority="5" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
@@ -3745,7 +4730,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M41:M42">
+  <conditionalFormatting sqref="M50:M51">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
@@ -3753,7 +4738,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M44:M45">
+  <conditionalFormatting sqref="M53:M54">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>

</xml_diff>